<commit_message>
Add ui and ux
</commit_message>
<xml_diff>
--- a/server/output/members.xlsx
+++ b/server/output/members.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -418,6 +418,12 @@
       <c r="E1" t="str">
         <v>photo</v>
       </c>
+      <c r="F1" t="str">
+        <v>id</v>
+      </c>
+      <c r="G1" t="str">
+        <v>createdAt</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -436,9 +442,95 @@
         <v>uploads/abcd_1752061505519.jpeg</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Abu Inshah</v>
+      </c>
+      <c r="B3" t="str">
+        <v>7449085120</v>
+      </c>
+      <c r="C3" t="str">
+        <v>ajai17101999@gmail.com</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Health insurance advisor</v>
+      </c>
+      <c r="E3" t="str">
+        <v>uploads/abu_inshah_1752306015359.jpeg</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>ram</v>
+      </c>
+      <c r="B4" t="str">
+        <v>7449085120</v>
+      </c>
+      <c r="C4" t="str">
+        <v>aiautomationhig@gmail.com</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Health insurance advisor</v>
+      </c>
+      <c r="E4" t="str">
+        <v>uploads/ram_1752311161933.jpeg</v>
+      </c>
+      <c r="F4" t="str">
+        <v>1752311162001</v>
+      </c>
+      <c r="G4" t="str">
+        <v>2025-07-12T09:06:02.001Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>ram</v>
+      </c>
+      <c r="B5" t="str">
+        <v>7449085120</v>
+      </c>
+      <c r="C5" t="str">
+        <v>selvasuresh460@gmail.com</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Health insurance advisor</v>
+      </c>
+      <c r="E5" t="str">
+        <v>uploads/ram_1752314093239.jpeg</v>
+      </c>
+      <c r="F5" t="str">
+        <v>1752314093256</v>
+      </c>
+      <c r="G5" t="str">
+        <v>2025-07-12T09:54:53.256Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Abu Inshah</v>
+      </c>
+      <c r="B6" t="str">
+        <v>7449085120</v>
+      </c>
+      <c r="C6" t="str">
+        <v>wealthplusacademy@gmail.com</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Wealth Manager</v>
+      </c>
+      <c r="E6" t="str">
+        <v>uploads/abu_inshah_1752314719383.jpeg</v>
+      </c>
+      <c r="F6" t="str">
+        <v>1752314719399</v>
+      </c>
+      <c r="G6" t="str">
+        <v>2025-07-12T10:05:19.399Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>